<commit_message>
Se agrega funcionalidad para adicionar a la estructura Json del ejercicio WriteActivity la traducción de la frase
</commit_message>
<xml_diff>
--- a/ImageWordActivity/Resources/Actividad-imagen-palabra.xlsx
+++ b/ImageWordActivity/Resources/Actividad-imagen-palabra.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>Eres,tanta,gente,quién,ahora</t>
   </si>
@@ -542,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +610,104 @@
       </c>
       <c r="D4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualizan excel y JSON
</commit_message>
<xml_diff>
--- a/ImageWordActivity/Resources/Actividad-imagen-palabra.xlsx
+++ b/ImageWordActivity/Resources/Actividad-imagen-palabra.xlsx
@@ -113,10 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
-  <si>
-    <t>Eres,tanta,gente,quién,ahora</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Nivel</t>
   </si>
@@ -124,34 +121,100 @@
     <t>Palabras a mostrar</t>
   </si>
   <si>
-    <t>Eres</t>
-  </si>
-  <si>
     <t>Traduccion</t>
   </si>
   <si>
     <t>Palabra valida</t>
   </si>
   <si>
-    <t>Pronto</t>
-  </si>
-  <si>
-    <t>Pronto,habilidad,casa</t>
-  </si>
-  <si>
-    <t>Cualidad,todos,vamos</t>
-  </si>
-  <si>
-    <t>todos</t>
-  </si>
-  <si>
-    <t>Prontoss</t>
-  </si>
-  <si>
-    <t>todoss</t>
-  </si>
-  <si>
-    <t>Eress</t>
+    <t>ABUELO</t>
+  </si>
+  <si>
+    <t>MANOS</t>
+  </si>
+  <si>
+    <t>FLORES</t>
+  </si>
+  <si>
+    <t>CAMINO</t>
+  </si>
+  <si>
+    <t>SOMBRERO</t>
+  </si>
+  <si>
+    <t>maki</t>
+  </si>
+  <si>
+    <t>MAIZ</t>
+  </si>
+  <si>
+    <t>HIJAS</t>
+  </si>
+  <si>
+    <t>Ushi</t>
+  </si>
+  <si>
+    <t>Sisa</t>
+  </si>
+  <si>
+    <t>Ñan</t>
+  </si>
+  <si>
+    <t>Muchiju</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTAÑA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urku /Urcu </t>
+  </si>
+  <si>
+    <t>VER</t>
+  </si>
+  <si>
+    <t>Rricuy / Rikuna</t>
+  </si>
+  <si>
+    <t>Sara / Zara</t>
+  </si>
+  <si>
+    <t>Ushtacuna /Ushutacuna</t>
+  </si>
+  <si>
+    <t>maki, Alpa/ Allpa, Pungu / Punku, Samanawasi, Puca/Puka</t>
+  </si>
+  <si>
+    <t>Rricuy / Rikuna, Cucha/Kucha , Atalpa/Atallpa, Kaspi, Ñuca/Ñuka</t>
+  </si>
+  <si>
+    <t>Ushi, Maki, Sara, Wasi, Runa</t>
+  </si>
+  <si>
+    <t>Sara / Zara,  Urpigo/ Urpiku, Wasigo/ Wasiku, Jachun/Hachun, Llacta /Llakta</t>
+  </si>
+  <si>
+    <t>ZAPATOS (ALPARGATES)</t>
+  </si>
+  <si>
+    <t>Sisa, Kaspi, wawa, shimi, Uma</t>
+  </si>
+  <si>
+    <t>Ñan, Maki, Uma, Kamya, Sara</t>
+  </si>
+  <si>
+    <t>Muchiju, Shimi,  Wagra, Killu, Yana</t>
+  </si>
+  <si>
+    <t>Ushtacuna /Ushutacuna, Pamba/pampa, Curi/Kuri, Cucha/ Kucha, Jawa/Hawa, Rricuy/Ricuna</t>
+  </si>
+  <si>
+    <t>Urku /Urcu,  Rrimay/Riman,  Jatun Taita/ Hatun Taita , Paycuna/Paykuna, Ñuca/Ñuka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jatun Taita /Hatun Taita </t>
+  </si>
+  <si>
+    <t>Jatun Taita /Hatun Taita,  Jatun Mama/Hatun Mama, Cucha/Kucha,  Jachun/Hachu, Curi/Kuri</t>
   </si>
 </sst>
 </file>
@@ -234,13 +297,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,6 +314,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -545,29 +612,29 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -575,139 +642,139 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
+      <c r="B4" t="s">
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
+      <c r="B6" t="s">
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
+      <c r="B7" t="s">
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
+      <c r="B11" t="s">
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>